<commit_message>
Back to school 2022
</commit_message>
<xml_diff>
--- a/220321_TUV_test_conditions.xlsx
+++ b/220321_TUV_test_conditions.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BU05\Dropbox (DualSun)\BU01-Industrialisation\01-Produit\01-Elements_thermiques\01-Echangeur thermique\XX-Etudes techniques\03-Performance test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\PVT-perf-1Dmodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5C20F5-27B1-4F54-83A6-AAFCD883D309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848705C1-47EF-4660-92E2-93293616454C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A02FE2B-2717-4255-A09B-CD64A0D733A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6A02FE2B-2717-4255-A09B-CD64A0D733A8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Non insulated v4 TUV" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Non insulated v4 TUV G=0" sheetId="6" r:id="rId2"/>
     <sheet name="Insulated v4 TUV" sheetId="5" r:id="rId3"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -216,9 +216,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -386,11 +386,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -898,30 +898,30 @@
         <v>0.41399999999999998</v>
       </c>
       <c r="N3">
-        <f>L3/'Non insulated v4 TUV'!$X$1</f>
+        <f>L3/Data!$X$1</f>
         <v>400.15487867836862</v>
       </c>
       <c r="P3">
         <v>966</v>
       </c>
       <c r="Q3">
-        <f>J3</f>
+        <f t="shared" ref="Q3:Q20" si="0">J3</f>
         <v>-1.39</v>
       </c>
       <c r="R3">
-        <f>Q3^2</f>
+        <f t="shared" ref="R3:R20" si="1">Q3^2</f>
         <v>1.9320999999999997</v>
       </c>
       <c r="S3">
-        <f>(E3-3)*Q3</f>
+        <f t="shared" ref="S3:S20" si="2">(E3-3)*Q3</f>
         <v>3.1969999999999996</v>
       </c>
       <c r="T3">
-        <f>(E3-3)*C3</f>
+        <f t="shared" ref="T3:T20" si="3">(E3-3)*C3</f>
         <v>-2221.7999999999997</v>
       </c>
       <c r="U3">
-        <f>+Q3^4</f>
+        <f t="shared" ref="U3:U20" si="4">+Q3^4</f>
         <v>3.733010409999999</v>
       </c>
       <c r="W3" s="3" t="s">
@@ -985,31 +985,31 @@
         <v>0.41599999999999998</v>
       </c>
       <c r="N4">
-        <f>L4/'Non insulated v4 TUV'!$X$1</f>
+        <f>L4/Data!$X$1</f>
         <v>401.65203923593185</v>
       </c>
       <c r="P4">
-        <f>C4</f>
+        <f t="shared" ref="P4:P20" si="5">C4</f>
         <v>966</v>
       </c>
       <c r="Q4">
-        <f>J4</f>
+        <f t="shared" si="0"/>
         <v>-1.35</v>
       </c>
       <c r="R4">
-        <f>Q4^2</f>
+        <f t="shared" si="1"/>
         <v>1.8225000000000002</v>
       </c>
       <c r="S4">
-        <f>(E4-3)*Q4</f>
+        <f t="shared" si="2"/>
         <v>3.105</v>
       </c>
       <c r="T4">
-        <f>(E4-3)*C4</f>
+        <f t="shared" si="3"/>
         <v>-2221.7999999999997</v>
       </c>
       <c r="U4">
-        <f>+Q4^4</f>
+        <f t="shared" si="4"/>
         <v>3.321506250000001</v>
       </c>
       <c r="W4" s="6" t="s">
@@ -1073,31 +1073,31 @@
         <v>0.38900000000000001</v>
       </c>
       <c r="N5">
-        <f>L5/'Non insulated v4 TUV'!$X$1</f>
+        <f>L5/Data!$X$1</f>
         <v>376.20030975735676</v>
       </c>
       <c r="P5">
-        <f>C5</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q5">
-        <f>J5</f>
+        <f t="shared" si="0"/>
         <v>-0.63</v>
       </c>
       <c r="R5">
-        <f>Q5^2</f>
+        <f t="shared" si="1"/>
         <v>0.39690000000000003</v>
       </c>
       <c r="S5">
-        <f>(E5-3)*Q5</f>
+        <f t="shared" si="2"/>
         <v>1.008</v>
       </c>
       <c r="T5">
-        <f>(E5-3)*C5</f>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="U5">
-        <f>+Q5^4</f>
+        <f t="shared" si="4"/>
         <v>0.15752961000000001</v>
       </c>
       <c r="W5" s="9" cm="1">
@@ -1164,31 +1164,31 @@
         <v>0.38800000000000001</v>
       </c>
       <c r="N6">
-        <f>L6/'Non insulated v4 TUV'!$X$1</f>
+        <f>L6/Data!$X$1</f>
         <v>375.11615900877644</v>
       </c>
       <c r="P6">
-        <f>C6</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q6">
-        <f>J6</f>
+        <f t="shared" si="0"/>
         <v>-0.43</v>
       </c>
       <c r="R6">
-        <f>Q6^2</f>
+        <f t="shared" si="1"/>
         <v>0.18489999999999998</v>
       </c>
       <c r="S6">
-        <f>(E6-3)*Q6</f>
+        <f t="shared" si="2"/>
         <v>0.68800000000000006</v>
       </c>
       <c r="T6">
-        <f>(E6-3)*C6</f>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="U6">
-        <f>+Q6^4</f>
+        <f t="shared" si="4"/>
         <v>3.4188009999999991E-2</v>
       </c>
       <c r="W6" s="6">
@@ -1254,31 +1254,31 @@
         <v>0.34300000000000003</v>
       </c>
       <c r="N7">
-        <f>L7/'Non insulated v4 TUV'!$X$1</f>
+        <f>L7/Data!$X$1</f>
         <v>331.75012906556532</v>
       </c>
       <c r="P7">
-        <f>C7</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q7">
-        <f>J7</f>
+        <f t="shared" si="0"/>
         <v>-0.03</v>
       </c>
       <c r="R7">
-        <f>Q7^2</f>
+        <f t="shared" si="1"/>
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="S7">
-        <f>(E7-3)*Q7</f>
+        <f t="shared" si="2"/>
         <v>8.9999999999999941E-3</v>
       </c>
       <c r="T7">
-        <f>(E7-3)*C7</f>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="U7">
-        <f>+Q7^4</f>
+        <f t="shared" si="4"/>
         <v>8.0999999999999997E-7</v>
       </c>
       <c r="W7" s="16">
@@ -1344,31 +1344,31 @@
         <v>0.34200000000000003</v>
       </c>
       <c r="N8">
-        <f>L8/'Non insulated v4 TUV'!$X$1</f>
+        <f>L8/Data!$X$1</f>
         <v>330.66597831698505</v>
       </c>
       <c r="P8">
-        <f>C8</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q8">
-        <f>J8</f>
+        <f t="shared" si="0"/>
         <v>-0.14000000000000001</v>
       </c>
       <c r="R8">
-        <f>Q8^2</f>
+        <f t="shared" si="1"/>
         <v>1.9600000000000003E-2</v>
       </c>
       <c r="S8">
-        <f>(E8-3)*Q8</f>
+        <f t="shared" si="2"/>
         <v>4.1999999999999982E-2</v>
       </c>
       <c r="T8">
-        <f>(E8-3)*C8</f>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="U8">
-        <f>+Q8^4</f>
+        <f t="shared" si="4"/>
         <v>3.8416000000000009E-4</v>
       </c>
       <c r="W8" s="6">
@@ -1434,31 +1434,31 @@
         <v>0.34200000000000003</v>
       </c>
       <c r="N9">
-        <f>L9/'Non insulated v4 TUV'!$X$1</f>
+        <f>L9/Data!$X$1</f>
         <v>330.30459473412492</v>
       </c>
       <c r="P9">
-        <f>C9</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q9">
-        <f>J9</f>
+        <f t="shared" si="0"/>
         <v>6.06</v>
       </c>
       <c r="R9">
-        <f>Q9^2</f>
+        <f t="shared" si="1"/>
         <v>36.723599999999998</v>
       </c>
       <c r="S9">
-        <f>(E9-3)*Q9</f>
+        <f t="shared" si="2"/>
         <v>-13.937999999999999</v>
       </c>
       <c r="T9">
-        <f>(E9-3)*C9</f>
+        <f t="shared" si="3"/>
         <v>-2221.7999999999997</v>
       </c>
       <c r="U9">
-        <f>+Q9^4</f>
+        <f t="shared" si="4"/>
         <v>1348.6227969599997</v>
       </c>
       <c r="W9" s="13">
@@ -1524,31 +1524,31 @@
         <v>0.34200000000000003</v>
       </c>
       <c r="N10">
-        <f>L10/'Non insulated v4 TUV'!$X$1</f>
+        <f>L10/Data!$X$1</f>
         <v>330.35622096024781</v>
       </c>
       <c r="P10">
-        <f>C10</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q10">
-        <f>J10</f>
+        <f t="shared" si="0"/>
         <v>6.11</v>
       </c>
       <c r="R10">
-        <f>Q10^2</f>
+        <f t="shared" si="1"/>
         <v>37.332100000000004</v>
       </c>
       <c r="S10">
-        <f>(E10-3)*Q10</f>
+        <f t="shared" si="2"/>
         <v>-14.052999999999999</v>
       </c>
       <c r="T10">
-        <f>(E10-3)*C10</f>
+        <f t="shared" si="3"/>
         <v>-2221.7999999999997</v>
       </c>
       <c r="U10">
-        <f>+Q10^4</f>
+        <f t="shared" si="4"/>
         <v>1393.6856904100002</v>
       </c>
     </row>
@@ -1593,31 +1593,31 @@
         <v>0.30499999999999999</v>
       </c>
       <c r="N11">
-        <f>L11/'Non insulated v4 TUV'!$X$1</f>
+        <f>L11/Data!$X$1</f>
         <v>294.83737738771293</v>
       </c>
       <c r="P11">
-        <f>C11</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q11">
-        <f>J11</f>
+        <f t="shared" si="0"/>
         <v>6.95</v>
       </c>
       <c r="R11">
-        <f>Q11^2</f>
+        <f t="shared" si="1"/>
         <v>48.302500000000002</v>
       </c>
       <c r="S11">
-        <f>(E11-3)*Q11</f>
+        <f t="shared" si="2"/>
         <v>-11.120000000000001</v>
       </c>
       <c r="T11">
-        <f>(E11-3)*C11</f>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="U11">
-        <f>+Q11^4</f>
+        <f t="shared" si="4"/>
         <v>2333.1315062500003</v>
       </c>
     </row>
@@ -1662,31 +1662,31 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="N12">
-        <f>L12/'Non insulated v4 TUV'!$X$1</f>
+        <f>L12/Data!$X$1</f>
         <v>295.76664945792459</v>
       </c>
       <c r="P12">
-        <f>C12</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q12">
-        <f>J12</f>
+        <f t="shared" si="0"/>
         <v>6.79</v>
       </c>
       <c r="R12">
-        <f>Q12^2</f>
+        <f t="shared" si="1"/>
         <v>46.104100000000003</v>
       </c>
       <c r="S12">
-        <f>(E12-3)*Q12</f>
+        <f t="shared" si="2"/>
         <v>-10.864000000000001</v>
       </c>
       <c r="T12">
-        <f>(E12-3)*C12</f>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="U12">
-        <f>+Q12^4</f>
+        <f t="shared" si="4"/>
         <v>2125.5880368100002</v>
       </c>
       <c r="W12">
@@ -1735,31 +1735,31 @@
         <v>0.247</v>
       </c>
       <c r="N13">
-        <f>L13/'Non insulated v4 TUV'!$X$1</f>
+        <f>L13/Data!$X$1</f>
         <v>238.51316468766132</v>
       </c>
       <c r="P13">
-        <f>C13</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q13">
-        <f>J13</f>
+        <f t="shared" si="0"/>
         <v>7.23</v>
       </c>
       <c r="R13">
-        <f>Q13^2</f>
+        <f t="shared" si="1"/>
         <v>52.272900000000007</v>
       </c>
       <c r="S13">
-        <f>(E13-3)*Q13</f>
+        <f t="shared" si="2"/>
         <v>-2.1689999999999987</v>
       </c>
       <c r="T13">
-        <f>(E13-3)*C13</f>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="U13">
-        <f>+Q13^4</f>
+        <f t="shared" si="4"/>
         <v>2732.4560744100008</v>
       </c>
     </row>
@@ -1804,31 +1804,31 @@
         <v>0.248</v>
       </c>
       <c r="N14">
-        <f>L14/'Non insulated v4 TUV'!$X$1</f>
+        <f>L14/Data!$X$1</f>
         <v>239.28755807950438</v>
       </c>
       <c r="P14">
-        <f>C14</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q14">
-        <f>J14</f>
+        <f t="shared" si="0"/>
         <v>7.23</v>
       </c>
       <c r="R14">
-        <f>Q14^2</f>
+        <f t="shared" si="1"/>
         <v>52.272900000000007</v>
       </c>
       <c r="S14">
-        <f>(E14-3)*Q14</f>
+        <f t="shared" si="2"/>
         <v>-2.1689999999999987</v>
       </c>
       <c r="T14">
-        <f>(E14-3)*C14</f>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="U14">
-        <f>+Q14^4</f>
+        <f t="shared" si="4"/>
         <v>2732.4560744100008</v>
       </c>
     </row>
@@ -1873,31 +1873,31 @@
         <v>0.252</v>
       </c>
       <c r="N15">
-        <f>L15/'Non insulated v4 TUV'!$X$1</f>
+        <f>L15/Data!$X$1</f>
         <v>243.21115126484256</v>
       </c>
       <c r="P15">
-        <f>C15</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q15">
-        <f>J15</f>
+        <f t="shared" si="0"/>
         <v>14.97</v>
       </c>
       <c r="R15">
-        <f>Q15^2</f>
+        <f t="shared" si="1"/>
         <v>224.10090000000002</v>
       </c>
       <c r="S15">
-        <f>(E15-3)*Q15</f>
+        <f t="shared" si="2"/>
         <v>-34.430999999999997</v>
       </c>
       <c r="T15">
-        <f>(E15-3)*C15</f>
+        <f t="shared" si="3"/>
         <v>-2221.7999999999997</v>
       </c>
       <c r="U15">
-        <f>+Q15^4</f>
+        <f t="shared" si="4"/>
         <v>50221.213380810012</v>
       </c>
     </row>
@@ -1942,31 +1942,31 @@
         <v>0.252</v>
       </c>
       <c r="N16">
-        <f>L16/'Non insulated v4 TUV'!$X$1</f>
+        <f>L16/Data!$X$1</f>
         <v>243.88229220443984</v>
       </c>
       <c r="P16">
-        <f>C16</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q16">
-        <f>J16</f>
+        <f t="shared" si="0"/>
         <v>14.8</v>
       </c>
       <c r="R16">
-        <f>Q16^2</f>
+        <f t="shared" si="1"/>
         <v>219.04000000000002</v>
       </c>
       <c r="S16">
-        <f>(E16-3)*Q16</f>
+        <f t="shared" si="2"/>
         <v>-34.04</v>
       </c>
       <c r="T16">
-        <f>(E16-3)*C16</f>
+        <f t="shared" si="3"/>
         <v>-2221.7999999999997</v>
       </c>
       <c r="U16">
-        <f>+Q16^4</f>
+        <f t="shared" si="4"/>
         <v>47978.521600000007</v>
       </c>
     </row>
@@ -2011,31 +2011,31 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="N17">
-        <f>L17/'Non insulated v4 TUV'!$X$1</f>
+        <f>L17/Data!$X$1</f>
         <v>197.88332472896232</v>
       </c>
       <c r="P17">
-        <f>C17</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q17">
-        <f>J17</f>
+        <f t="shared" si="0"/>
         <v>15.74</v>
       </c>
       <c r="R17">
-        <f>Q17^2</f>
+        <f t="shared" si="1"/>
         <v>247.74760000000001</v>
       </c>
       <c r="S17">
-        <f>(E17-3)*Q17</f>
+        <f t="shared" si="2"/>
         <v>-25.184000000000001</v>
       </c>
       <c r="T17">
-        <f>(E17-3)*C17</f>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="U17">
-        <f>+Q17^4</f>
+        <f t="shared" si="4"/>
         <v>61378.873305760004</v>
       </c>
     </row>
@@ -2080,31 +2080,31 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="N18">
-        <f>L18/'Non insulated v4 TUV'!$X$1</f>
+        <f>L18/Data!$X$1</f>
         <v>198.29633453794528</v>
       </c>
       <c r="P18">
-        <f>C18</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q18">
-        <f>J18</f>
+        <f t="shared" si="0"/>
         <v>15.65</v>
       </c>
       <c r="R18">
-        <f>Q18^2</f>
+        <f t="shared" si="1"/>
         <v>244.92250000000001</v>
       </c>
       <c r="S18">
-        <f>(E18-3)*Q18</f>
+        <f t="shared" si="2"/>
         <v>-25.040000000000003</v>
       </c>
       <c r="T18">
-        <f>(E18-3)*C18</f>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="U18">
-        <f>+Q18^4</f>
+        <f t="shared" si="4"/>
         <v>59987.031006250007</v>
       </c>
     </row>
@@ -2149,31 +2149,31 @@
         <v>0.127</v>
       </c>
       <c r="N19">
-        <f>L19/'Non insulated v4 TUV'!$X$1</f>
+        <f>L19/Data!$X$1</f>
         <v>122.71553949406298</v>
       </c>
       <c r="P19">
-        <f>C19</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q19">
-        <f>J19</f>
+        <f t="shared" si="0"/>
         <v>16.14</v>
       </c>
       <c r="R19">
-        <f>Q19^2</f>
+        <f t="shared" si="1"/>
         <v>260.49960000000004</v>
       </c>
       <c r="S19">
-        <f>(E19-3)*Q19</f>
+        <f t="shared" si="2"/>
         <v>-4.841999999999997</v>
       </c>
       <c r="T19">
-        <f>(E19-3)*C19</f>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="U19">
-        <f>+Q19^4</f>
+        <f t="shared" si="4"/>
         <v>67860.041600160024</v>
       </c>
     </row>
@@ -2218,31 +2218,31 @@
         <v>0.127</v>
       </c>
       <c r="N20">
-        <f>L20/'Non insulated v4 TUV'!$X$1</f>
+        <f>L20/Data!$X$1</f>
         <v>122.8704181724316</v>
       </c>
       <c r="P20">
-        <f>C20</f>
+        <f t="shared" si="5"/>
         <v>966</v>
       </c>
       <c r="Q20">
-        <f>J20</f>
+        <f t="shared" si="0"/>
         <v>16.18</v>
       </c>
       <c r="R20">
-        <f>Q20^2</f>
+        <f t="shared" si="1"/>
         <v>261.79239999999999</v>
       </c>
       <c r="S20">
-        <f>(E20-3)*Q20</f>
+        <f t="shared" si="2"/>
         <v>-4.8539999999999974</v>
       </c>
       <c r="T20">
-        <f>(E20-3)*C20</f>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="U20">
-        <f>+Q20^4</f>
+        <f t="shared" si="4"/>
         <v>68535.260697759993</v>
       </c>
     </row>
@@ -2384,31 +2384,31 @@
         <v>31.4</v>
       </c>
       <c r="N3">
-        <f>L3/'Non insulated v4 TUV'!$X$1</f>
+        <f>L3/Data!$X$1</f>
         <v>16.210635002581309</v>
       </c>
       <c r="P3">
-        <f>C3</f>
+        <f t="shared" ref="P3:P33" si="0">C3</f>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f>J3</f>
+        <f t="shared" ref="Q3:Q33" si="1">J3</f>
         <v>-2.0499999999999998</v>
       </c>
       <c r="R3">
-        <f>Q3^2</f>
+        <f t="shared" ref="R3:R33" si="2">Q3^2</f>
         <v>4.2024999999999997</v>
       </c>
       <c r="S3">
-        <f>(E3-3)*Q3</f>
+        <f t="shared" ref="S3:S33" si="3">(E3-3)*Q3</f>
         <v>4.51</v>
       </c>
       <c r="T3">
-        <f>(E3-3)*C3</f>
+        <f t="shared" ref="T3:T33" si="4">(E3-3)*C3</f>
         <v>0</v>
       </c>
       <c r="U3">
-        <f>+Q3^4</f>
+        <f t="shared" ref="U3:U33" si="5">+Q3^4</f>
         <v>17.661006249999996</v>
       </c>
     </row>
@@ -2450,31 +2450,31 @@
         <v>31.3</v>
       </c>
       <c r="N4">
-        <f>L4/'Non insulated v4 TUV'!$X$1</f>
+        <f>L4/Data!$X$1</f>
         <v>16.159008776458442</v>
       </c>
       <c r="P4">
-        <f>C4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f>J4</f>
+        <f t="shared" si="1"/>
         <v>-2.04</v>
       </c>
       <c r="R4">
-        <f>Q4^2</f>
+        <f t="shared" si="2"/>
         <v>4.1616</v>
       </c>
       <c r="S4">
-        <f>(E4-3)*Q4</f>
+        <f t="shared" si="3"/>
         <v>4.4880000000000004</v>
       </c>
       <c r="T4">
-        <f>(E4-3)*C4</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U4">
-        <f>+Q4^4</f>
+        <f t="shared" si="5"/>
         <v>17.31891456</v>
       </c>
     </row>
@@ -2516,31 +2516,31 @@
         <v>37.799999999999997</v>
       </c>
       <c r="N5">
-        <f>L5/'Non insulated v4 TUV'!$X$1</f>
+        <f>L5/Data!$X$1</f>
         <v>19.514713474445017</v>
       </c>
       <c r="P5">
-        <f>C5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q5">
-        <f>J5</f>
+        <f t="shared" si="1"/>
         <v>-2.15</v>
       </c>
       <c r="R5">
-        <f>Q5^2</f>
+        <f t="shared" si="2"/>
         <v>4.6224999999999996</v>
       </c>
       <c r="S5">
-        <f>(E5-3)*Q5</f>
+        <f t="shared" si="3"/>
         <v>3.01</v>
       </c>
       <c r="T5">
-        <f>(E5-3)*C5</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U5">
-        <f>+Q5^4</f>
+        <f t="shared" si="5"/>
         <v>21.367506249999998</v>
       </c>
     </row>
@@ -2582,31 +2582,31 @@
         <v>38.299999999999997</v>
       </c>
       <c r="N6">
-        <f>L6/'Non insulated v4 TUV'!$X$1</f>
+        <f>L6/Data!$X$1</f>
         <v>19.772844605059369</v>
       </c>
       <c r="P6">
-        <f>C6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f>J6</f>
+        <f t="shared" si="1"/>
         <v>-2.14</v>
       </c>
       <c r="R6">
-        <f>Q6^2</f>
+        <f t="shared" si="2"/>
         <v>4.5796000000000001</v>
       </c>
       <c r="S6">
-        <f>(E6-3)*Q6</f>
+        <f t="shared" si="3"/>
         <v>2.996</v>
       </c>
       <c r="T6">
-        <f>(E6-3)*C6</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U6">
-        <f>+Q6^4</f>
+        <f t="shared" si="5"/>
         <v>20.97273616</v>
       </c>
     </row>
@@ -2648,31 +2648,31 @@
         <v>45.7</v>
       </c>
       <c r="N7">
-        <f>L7/'Non insulated v4 TUV'!$X$1</f>
+        <f>L7/Data!$X$1</f>
         <v>23.59318533815178</v>
       </c>
       <c r="P7">
-        <f>C7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>J7</f>
+        <f t="shared" si="1"/>
         <v>-2.02</v>
       </c>
       <c r="R7">
-        <f>Q7^2</f>
+        <f t="shared" si="2"/>
         <v>4.0804</v>
       </c>
       <c r="S7">
-        <f>(E7-3)*Q7</f>
+        <f t="shared" si="3"/>
         <v>0.40400000000000036</v>
       </c>
       <c r="T7">
-        <f>(E7-3)*C7</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U7">
-        <f>+Q7^4</f>
+        <f t="shared" si="5"/>
         <v>16.64966416</v>
       </c>
     </row>
@@ -2714,31 +2714,31 @@
         <v>44.6</v>
       </c>
       <c r="N8">
-        <f>L8/'Non insulated v4 TUV'!$X$1</f>
+        <f>L8/Data!$X$1</f>
         <v>23.025296850800206</v>
       </c>
       <c r="P8">
-        <f>C8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f>J8</f>
+        <f t="shared" si="1"/>
         <v>-2.0299999999999998</v>
       </c>
       <c r="R8">
-        <f>Q8^2</f>
+        <f t="shared" si="2"/>
         <v>4.1208999999999989</v>
       </c>
       <c r="S8">
-        <f>(E8-3)*Q8</f>
+        <f t="shared" si="3"/>
         <v>0.40600000000000031</v>
       </c>
       <c r="T8">
-        <f>(E8-3)*C8</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U8">
-        <f>+Q8^4</f>
+        <f t="shared" si="5"/>
         <v>16.981816809999991</v>
       </c>
     </row>
@@ -2780,31 +2780,31 @@
         <v>-14.2</v>
       </c>
       <c r="N9">
-        <f>L9/'Non insulated v4 TUV'!$X$1</f>
+        <f>L9/Data!$X$1</f>
         <v>-7.330924109447599</v>
       </c>
       <c r="P9">
-        <f>C9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f>J9</f>
+        <f t="shared" si="1"/>
         <v>0.85</v>
       </c>
       <c r="R9">
-        <f>Q9^2</f>
+        <f t="shared" si="2"/>
         <v>0.72249999999999992</v>
       </c>
       <c r="S9">
-        <f>(E9-3)*Q9</f>
+        <f t="shared" si="3"/>
         <v>-1.87</v>
       </c>
       <c r="T9">
-        <f>(E9-3)*C9</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U9">
-        <f>+Q9^4</f>
+        <f t="shared" si="5"/>
         <v>0.52200624999999989</v>
       </c>
     </row>
@@ -2846,31 +2846,31 @@
         <v>-12.9</v>
       </c>
       <c r="N10">
-        <f>L10/'Non insulated v4 TUV'!$X$1</f>
+        <f>L10/Data!$X$1</f>
         <v>-6.6597831698502841</v>
       </c>
       <c r="P10">
-        <f>C10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f>J10</f>
+        <f t="shared" si="1"/>
         <v>0.83</v>
       </c>
       <c r="R10">
-        <f>Q10^2</f>
+        <f t="shared" si="2"/>
         <v>0.68889999999999996</v>
       </c>
       <c r="S10">
-        <f>(E10-3)*Q10</f>
+        <f t="shared" si="3"/>
         <v>-1.8260000000000001</v>
       </c>
       <c r="T10">
-        <f>(E10-3)*C10</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U10">
-        <f>+Q10^4</f>
+        <f t="shared" si="5"/>
         <v>0.47458320999999992</v>
       </c>
     </row>
@@ -2912,31 +2912,31 @@
         <v>-12.4</v>
       </c>
       <c r="N11">
-        <f>L11/'Non insulated v4 TUV'!$X$1</f>
+        <f>L11/Data!$X$1</f>
         <v>-6.4016520392359322</v>
       </c>
       <c r="P11">
-        <f>C11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f>J11</f>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="R11">
-        <f>Q11^2</f>
+        <f t="shared" si="2"/>
         <v>0.5625</v>
       </c>
       <c r="S11">
-        <f>(E11-3)*Q11</f>
+        <f t="shared" si="3"/>
         <v>-1.0499999999999998</v>
       </c>
       <c r="T11">
-        <f>(E11-3)*C11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U11">
-        <f>+Q11^4</f>
+        <f t="shared" si="5"/>
         <v>0.31640625</v>
       </c>
     </row>
@@ -2978,31 +2978,31 @@
         <v>-13.3</v>
       </c>
       <c r="N12">
-        <f>L12/'Non insulated v4 TUV'!$X$1</f>
+        <f>L12/Data!$X$1</f>
         <v>-6.8662880743417656</v>
       </c>
       <c r="P12">
-        <f>C12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>J12</f>
+        <f t="shared" si="1"/>
         <v>0.79</v>
       </c>
       <c r="R12">
-        <f>Q12^2</f>
+        <f t="shared" si="2"/>
         <v>0.6241000000000001</v>
       </c>
       <c r="S12">
-        <f>(E12-3)*Q12</f>
+        <f t="shared" si="3"/>
         <v>-1.1059999999999999</v>
       </c>
       <c r="T12">
-        <f>(E12-3)*C12</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U12">
-        <f>+Q12^4</f>
+        <f t="shared" si="5"/>
         <v>0.38950081000000014</v>
       </c>
     </row>
@@ -3044,31 +3044,31 @@
         <v>-13</v>
       </c>
       <c r="N13">
-        <f>L13/'Non insulated v4 TUV'!$X$1</f>
+        <f>L13/Data!$X$1</f>
         <v>-6.7114093959731544</v>
       </c>
       <c r="P13">
-        <f>C13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>J13</f>
+        <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
       <c r="R13">
-        <f>Q13^2</f>
+        <f t="shared" si="2"/>
         <v>0.60840000000000005</v>
       </c>
       <c r="S13">
-        <f>(E13-3)*Q13</f>
+        <f t="shared" si="3"/>
         <v>-0.15600000000000014</v>
       </c>
       <c r="T13">
-        <f>(E13-3)*C13</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U13">
-        <f>+Q13^4</f>
+        <f t="shared" si="5"/>
         <v>0.37015056000000007</v>
       </c>
     </row>
@@ -3110,31 +3110,31 @@
         <v>-14.1</v>
       </c>
       <c r="N14">
-        <f>L14/'Non insulated v4 TUV'!$X$1</f>
+        <f>L14/Data!$X$1</f>
         <v>-7.2792978833247286</v>
       </c>
       <c r="P14">
-        <f>C14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f>J14</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="R14">
-        <f>Q14^2</f>
+        <f t="shared" si="2"/>
         <v>0.64000000000000012</v>
       </c>
       <c r="S14">
-        <f>(E14-3)*Q14</f>
+        <f t="shared" si="3"/>
         <v>-0.16000000000000014</v>
       </c>
       <c r="T14">
-        <f>(E14-3)*C14</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U14">
-        <f>+Q14^4</f>
+        <f t="shared" si="5"/>
         <v>0.40960000000000019</v>
       </c>
     </row>
@@ -3176,31 +3176,31 @@
         <v>-157.80000000000001</v>
       </c>
       <c r="N15">
-        <f>L15/'Non insulated v4 TUV'!$X$1</f>
+        <f>L15/Data!$X$1</f>
         <v>-81.466184821889527</v>
       </c>
       <c r="P15">
-        <f>C15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>J15</f>
+        <f t="shared" si="1"/>
         <v>9.15</v>
       </c>
       <c r="R15">
-        <f>Q15^2</f>
+        <f t="shared" si="2"/>
         <v>83.722500000000011</v>
       </c>
       <c r="S15">
-        <f>(E15-3)*Q15</f>
+        <f t="shared" si="3"/>
         <v>-20.130000000000003</v>
       </c>
       <c r="T15">
-        <f>(E15-3)*C15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U15">
-        <f>+Q15^4</f>
+        <f t="shared" si="5"/>
         <v>7009.4570062500015</v>
       </c>
     </row>
@@ -3242,31 +3242,31 @@
         <v>-156</v>
       </c>
       <c r="N16">
-        <f>L16/'Non insulated v4 TUV'!$X$1</f>
+        <f>L16/Data!$X$1</f>
         <v>-80.536912751677846</v>
       </c>
       <c r="P16">
-        <f>C16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f>J16</f>
+        <f t="shared" si="1"/>
         <v>9.1</v>
       </c>
       <c r="R16">
-        <f>Q16^2</f>
+        <f t="shared" si="2"/>
         <v>82.809999999999988</v>
       </c>
       <c r="S16">
-        <f>(E16-3)*Q16</f>
+        <f t="shared" si="3"/>
         <v>-20.02</v>
       </c>
       <c r="T16">
-        <f>(E16-3)*C16</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U16">
-        <f>+Q16^4</f>
+        <f t="shared" si="5"/>
         <v>6857.4960999999985</v>
       </c>
     </row>
@@ -3308,31 +3308,31 @@
         <v>-183.9</v>
       </c>
       <c r="N17">
-        <f>L17/'Non insulated v4 TUV'!$X$1</f>
+        <f>L17/Data!$X$1</f>
         <v>-94.940629839958703</v>
       </c>
       <c r="P17">
-        <f>C17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q17">
-        <f>J17</f>
+        <f t="shared" si="1"/>
         <v>8.74</v>
       </c>
       <c r="R17">
-        <f>Q17^2</f>
+        <f t="shared" si="2"/>
         <v>76.387600000000006</v>
       </c>
       <c r="S17">
-        <f>(E17-3)*Q17</f>
+        <f t="shared" si="3"/>
         <v>-12.235999999999999</v>
       </c>
       <c r="T17">
-        <f>(E17-3)*C17</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U17">
-        <f>+Q17^4</f>
+        <f t="shared" si="5"/>
         <v>5835.0654337600008</v>
       </c>
     </row>
@@ -3374,31 +3374,31 @@
         <v>-183.4</v>
       </c>
       <c r="N18">
-        <f>L18/'Non insulated v4 TUV'!$X$1</f>
+        <f>L18/Data!$X$1</f>
         <v>-94.682498709344344</v>
       </c>
       <c r="P18">
-        <f>C18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q18">
-        <f>J18</f>
+        <f t="shared" si="1"/>
         <v>8.7200000000000006</v>
       </c>
       <c r="R18">
-        <f>Q18^2</f>
+        <f t="shared" si="2"/>
         <v>76.03840000000001</v>
       </c>
       <c r="S18">
-        <f>(E18-3)*Q18</f>
+        <f t="shared" si="3"/>
         <v>-12.208</v>
       </c>
       <c r="T18">
-        <f>(E18-3)*C18</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U18">
-        <f>+Q18^4</f>
+        <f t="shared" si="5"/>
         <v>5781.8382745600011</v>
       </c>
     </row>
@@ -3440,31 +3440,31 @@
         <v>-208.7</v>
       </c>
       <c r="N19">
-        <f>L19/'Non insulated v4 TUV'!$X$1</f>
+        <f>L19/Data!$X$1</f>
         <v>-107.74393391843056</v>
       </c>
       <c r="P19">
-        <f>C19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q19">
-        <f>J19</f>
+        <f t="shared" si="1"/>
         <v>8.7899999999999991</v>
       </c>
       <c r="R19">
-        <f>Q19^2</f>
+        <f t="shared" si="2"/>
         <v>77.264099999999985</v>
       </c>
       <c r="S19">
-        <f>(E19-3)*Q19</f>
+        <f t="shared" si="3"/>
         <v>-1.7580000000000013</v>
       </c>
       <c r="T19">
-        <f>(E19-3)*C19</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U19">
-        <f>+Q19^4</f>
+        <f t="shared" si="5"/>
         <v>5969.7411488099979</v>
       </c>
     </row>
@@ -3506,31 +3506,31 @@
         <v>-208.3</v>
       </c>
       <c r="N20">
-        <f>L20/'Non insulated v4 TUV'!$X$1</f>
+        <f>L20/Data!$X$1</f>
         <v>-107.53742901393909</v>
       </c>
       <c r="P20">
-        <f>C20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q20">
-        <f>J20</f>
+        <f t="shared" si="1"/>
         <v>8.7799999999999994</v>
       </c>
       <c r="R20">
-        <f>Q20^2</f>
+        <f t="shared" si="2"/>
         <v>77.088399999999993</v>
       </c>
       <c r="S20">
-        <f>(E20-3)*Q20</f>
+        <f t="shared" si="3"/>
         <v>-1.7560000000000013</v>
       </c>
       <c r="T20">
-        <f>(E20-3)*C20</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U20">
-        <f>+Q20^4</f>
+        <f t="shared" si="5"/>
         <v>5942.6214145599988</v>
       </c>
     </row>
@@ -3572,31 +3572,31 @@
         <v>-324.5</v>
       </c>
       <c r="N21">
-        <f>L21/'Non insulated v4 TUV'!$X$1</f>
+        <f>L21/Data!$X$1</f>
         <v>-167.52710376871451</v>
       </c>
       <c r="P21">
-        <f>C21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q21">
-        <f>J21</f>
+        <f t="shared" si="1"/>
         <v>17.690000000000001</v>
       </c>
       <c r="R21">
-        <f>Q21^2</f>
+        <f t="shared" si="2"/>
         <v>312.93610000000007</v>
       </c>
       <c r="S21">
-        <f>(E21-3)*Q21</f>
+        <f t="shared" si="3"/>
         <v>-38.918000000000006</v>
       </c>
       <c r="T21">
-        <f>(E21-3)*C21</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U21">
-        <f>+Q21^4</f>
+        <f t="shared" si="5"/>
         <v>97929.002683210041</v>
       </c>
     </row>
@@ -3638,31 +3638,31 @@
         <v>-324.10000000000002</v>
       </c>
       <c r="N22">
-        <f>L22/'Non insulated v4 TUV'!$X$1</f>
+        <f>L22/Data!$X$1</f>
         <v>-167.32059886422303</v>
       </c>
       <c r="P22">
-        <f>C22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q22">
-        <f>J22</f>
+        <f t="shared" si="1"/>
         <v>17.670000000000002</v>
       </c>
       <c r="R22">
-        <f>Q22^2</f>
+        <f t="shared" si="2"/>
         <v>312.22890000000007</v>
       </c>
       <c r="S22">
-        <f>(E22-3)*Q22</f>
+        <f t="shared" si="3"/>
         <v>-38.874000000000009</v>
       </c>
       <c r="T22">
-        <f>(E22-3)*C22</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U22">
-        <f>+Q22^4</f>
+        <f t="shared" si="5"/>
         <v>97486.885995210047</v>
       </c>
     </row>
@@ -3704,31 +3704,31 @@
         <v>-370.8</v>
       </c>
       <c r="N23">
-        <f>L23/'Non insulated v4 TUV'!$X$1</f>
+        <f>L23/Data!$X$1</f>
         <v>-191.4300464636035</v>
       </c>
       <c r="P23">
-        <f>C23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q23">
-        <f>J23</f>
+        <f t="shared" si="1"/>
         <v>17.600000000000001</v>
       </c>
       <c r="R23">
-        <f>Q23^2</f>
+        <f t="shared" si="2"/>
         <v>309.76000000000005</v>
       </c>
       <c r="S23">
-        <f>(E23-3)*Q23</f>
+        <f t="shared" si="3"/>
         <v>-24.64</v>
       </c>
       <c r="T23">
-        <f>(E23-3)*C23</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U23">
-        <f>+Q23^4</f>
+        <f t="shared" si="5"/>
         <v>95951.257600000026</v>
       </c>
     </row>
@@ -3770,31 +3770,31 @@
         <v>-371.3</v>
       </c>
       <c r="N24">
-        <f>L24/'Non insulated v4 TUV'!$X$1</f>
+        <f>L24/Data!$X$1</f>
         <v>-191.68817759421788</v>
       </c>
       <c r="P24">
-        <f>C24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q24">
-        <f>J24</f>
+        <f t="shared" si="1"/>
         <v>17.579999999999998</v>
       </c>
       <c r="R24">
-        <f>Q24^2</f>
+        <f t="shared" si="2"/>
         <v>309.05639999999994</v>
       </c>
       <c r="S24">
-        <f>(E24-3)*Q24</f>
+        <f t="shared" si="3"/>
         <v>-24.611999999999995</v>
       </c>
       <c r="T24">
-        <f>(E24-3)*C24</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U24">
-        <f>+Q24^4</f>
+        <f t="shared" si="5"/>
         <v>95515.858380959966</v>
       </c>
     </row>
@@ -3836,31 +3836,31 @@
         <v>-419.9</v>
       </c>
       <c r="N25">
-        <f>L25/'Non insulated v4 TUV'!$X$1</f>
+        <f>L25/Data!$X$1</f>
         <v>-216.77852348993287</v>
       </c>
       <c r="P25">
-        <f>C25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q25">
-        <f>J25</f>
+        <f t="shared" si="1"/>
         <v>17.32</v>
       </c>
       <c r="R25">
-        <f>Q25^2</f>
+        <f t="shared" si="2"/>
         <v>299.98239999999998</v>
       </c>
       <c r="S25">
-        <f>(E25-3)*Q25</f>
+        <f t="shared" si="3"/>
         <v>-3.4640000000000031</v>
       </c>
       <c r="T25">
-        <f>(E25-3)*C25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U25">
-        <f>+Q25^4</f>
+        <f t="shared" si="5"/>
         <v>89989.440309759986</v>
       </c>
     </row>
@@ -3902,31 +3902,31 @@
         <v>-419.5</v>
       </c>
       <c r="N26">
-        <f>L26/'Non insulated v4 TUV'!$X$1</f>
+        <f>L26/Data!$X$1</f>
         <v>-216.57201858544138</v>
       </c>
       <c r="P26">
-        <f>C26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q26">
-        <f>J26</f>
+        <f t="shared" si="1"/>
         <v>17.309999999999999</v>
       </c>
       <c r="R26">
-        <f>Q26^2</f>
+        <f t="shared" si="2"/>
         <v>299.63609999999994</v>
       </c>
       <c r="S26">
-        <f>(E26-3)*Q26</f>
+        <f t="shared" si="3"/>
         <v>-3.4620000000000029</v>
       </c>
       <c r="T26">
-        <f>(E26-3)*C26</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U26">
-        <f>+Q26^4</f>
+        <f t="shared" si="5"/>
         <v>89781.792423209961</v>
       </c>
     </row>
@@ -3968,31 +3968,31 @@
         <v>-504.1</v>
       </c>
       <c r="N27">
-        <f>L27/'Non insulated v4 TUV'!$X$1</f>
+        <f>L27/Data!$X$1</f>
         <v>-260.24780588538977</v>
       </c>
       <c r="P27">
-        <f>C27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q27">
-        <f>J27</f>
+        <f t="shared" si="1"/>
         <v>26.36</v>
       </c>
       <c r="R27">
-        <f>Q27^2</f>
+        <f t="shared" si="2"/>
         <v>694.84960000000001</v>
       </c>
       <c r="S27">
-        <f>(E27-3)*Q27</f>
+        <f t="shared" si="3"/>
         <v>-57.992000000000004</v>
       </c>
       <c r="T27">
-        <f>(E27-3)*C27</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U27">
-        <f>+Q27^4</f>
+        <f t="shared" si="5"/>
         <v>482815.96662016003</v>
       </c>
     </row>
@@ -4034,31 +4034,31 @@
         <v>31.4</v>
       </c>
       <c r="N28">
-        <f>L28/'Non insulated v4 TUV'!$X$1</f>
+        <f>L28/Data!$X$1</f>
         <v>16.210635002581309</v>
       </c>
       <c r="P28">
-        <f>C28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q28">
-        <f>J28</f>
+        <f t="shared" si="1"/>
         <v>-2.0499999999999998</v>
       </c>
       <c r="R28">
-        <f>Q28^2</f>
+        <f t="shared" si="2"/>
         <v>4.2024999999999997</v>
       </c>
       <c r="S28">
-        <f>(E28-3)*Q28</f>
+        <f t="shared" si="3"/>
         <v>4.51</v>
       </c>
       <c r="T28">
-        <f>(E28-3)*C28</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U28">
-        <f>+Q28^4</f>
+        <f t="shared" si="5"/>
         <v>17.661006249999996</v>
       </c>
     </row>
@@ -4100,31 +4100,31 @@
         <v>31.3</v>
       </c>
       <c r="N29">
-        <f>L29/'Non insulated v4 TUV'!$X$1</f>
+        <f>L29/Data!$X$1</f>
         <v>16.159008776458442</v>
       </c>
       <c r="P29">
-        <f>C29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q29">
-        <f>J29</f>
+        <f t="shared" si="1"/>
         <v>-2.04</v>
       </c>
       <c r="R29">
-        <f>Q29^2</f>
+        <f t="shared" si="2"/>
         <v>4.1616</v>
       </c>
       <c r="S29">
-        <f>(E29-3)*Q29</f>
+        <f t="shared" si="3"/>
         <v>4.4880000000000004</v>
       </c>
       <c r="T29">
-        <f>(E29-3)*C29</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U29">
-        <f>+Q29^4</f>
+        <f t="shared" si="5"/>
         <v>17.31891456</v>
       </c>
     </row>
@@ -4166,31 +4166,31 @@
         <v>37.799999999999997</v>
       </c>
       <c r="N30">
-        <f>L30/'Non insulated v4 TUV'!$X$1</f>
+        <f>L30/Data!$X$1</f>
         <v>19.514713474445017</v>
       </c>
       <c r="P30">
-        <f>C30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q30">
-        <f>J30</f>
+        <f t="shared" si="1"/>
         <v>-2.15</v>
       </c>
       <c r="R30">
-        <f>Q30^2</f>
+        <f t="shared" si="2"/>
         <v>4.6224999999999996</v>
       </c>
       <c r="S30">
-        <f>(E30-3)*Q30</f>
+        <f t="shared" si="3"/>
         <v>3.01</v>
       </c>
       <c r="T30">
-        <f>(E30-3)*C30</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U30">
-        <f>+Q30^4</f>
+        <f t="shared" si="5"/>
         <v>21.367506249999998</v>
       </c>
     </row>
@@ -4232,31 +4232,31 @@
         <v>38.299999999999997</v>
       </c>
       <c r="N31">
-        <f>L31/'Non insulated v4 TUV'!$X$1</f>
+        <f>L31/Data!$X$1</f>
         <v>19.772844605059369</v>
       </c>
       <c r="P31">
-        <f>C31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q31">
-        <f>J31</f>
+        <f t="shared" si="1"/>
         <v>-2.14</v>
       </c>
       <c r="R31">
-        <f>Q31^2</f>
+        <f t="shared" si="2"/>
         <v>4.5796000000000001</v>
       </c>
       <c r="S31">
-        <f>(E31-3)*Q31</f>
+        <f t="shared" si="3"/>
         <v>2.996</v>
       </c>
       <c r="T31">
-        <f>(E31-3)*C31</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U31">
-        <f>+Q31^4</f>
+        <f t="shared" si="5"/>
         <v>20.97273616</v>
       </c>
     </row>
@@ -4298,31 +4298,31 @@
         <v>45.7</v>
       </c>
       <c r="N32">
-        <f>L32/'Non insulated v4 TUV'!$X$1</f>
+        <f>L32/Data!$X$1</f>
         <v>23.59318533815178</v>
       </c>
       <c r="P32">
-        <f>C32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q32">
-        <f>J32</f>
+        <f t="shared" si="1"/>
         <v>-2.02</v>
       </c>
       <c r="R32">
-        <f>Q32^2</f>
+        <f t="shared" si="2"/>
         <v>4.0804</v>
       </c>
       <c r="S32">
-        <f>(E32-3)*Q32</f>
+        <f t="shared" si="3"/>
         <v>0.40400000000000036</v>
       </c>
       <c r="T32">
-        <f>(E32-3)*C32</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U32">
-        <f>+Q32^4</f>
+        <f t="shared" si="5"/>
         <v>16.64966416</v>
       </c>
     </row>
@@ -4364,31 +4364,31 @@
         <v>44.6</v>
       </c>
       <c r="N33">
-        <f>L33/'Non insulated v4 TUV'!$X$1</f>
+        <f>L33/Data!$X$1</f>
         <v>23.025296850800206</v>
       </c>
       <c r="P33">
-        <f>C33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q33">
-        <f>J33</f>
+        <f t="shared" si="1"/>
         <v>-2.0299999999999998</v>
       </c>
       <c r="R33">
-        <f>Q33^2</f>
+        <f t="shared" si="2"/>
         <v>4.1208999999999989</v>
       </c>
       <c r="S33">
-        <f>(E33-3)*Q33</f>
+        <f t="shared" si="3"/>
         <v>0.40600000000000031</v>
       </c>
       <c r="T33">
-        <f>(E33-3)*C33</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U33">
-        <f>+Q33^4</f>
+        <f t="shared" si="5"/>
         <v>16.981816809999991</v>
       </c>
     </row>
@@ -4569,7 +4569,7 @@
         <v>0.41399999999999998</v>
       </c>
       <c r="N3">
-        <f>L3/'Non insulated v4 TUV'!$X$1</f>
+        <f>L3/Data!$X$1</f>
         <v>400.15487867836862</v>
       </c>
       <c r="P3">
@@ -4581,7 +4581,7 @@
         <v>-1.39</v>
       </c>
       <c r="R3">
-        <f>S3*Q3</f>
+        <f t="shared" ref="R3:R20" si="0">S3*Q3</f>
         <v>3088.3019999999992</v>
       </c>
       <c r="S3">
@@ -4650,27 +4650,27 @@
         <v>0.41599999999999998</v>
       </c>
       <c r="N4">
-        <f>L4/'Non insulated v4 TUV'!$X$1</f>
+        <f>L4/Data!$X$1</f>
         <v>401.65203923593185</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P20" si="0">C4</f>
+        <f t="shared" ref="P4:P20" si="1">C4</f>
         <v>966</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q20" si="1">J4</f>
+        <f t="shared" ref="Q4:Q20" si="2">J4</f>
         <v>-1.35</v>
       </c>
       <c r="R4">
-        <f>S4*Q4</f>
+        <f t="shared" si="0"/>
         <v>2999.43</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S20" si="2">(E4-3)*P4</f>
+        <f t="shared" ref="S4:S20" si="3">(E4-3)*P4</f>
         <v>-2221.7999999999997</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:T20" si="3">+Q4^4</f>
+        <f t="shared" ref="T4:T20" si="4">+Q4^4</f>
         <v>3.321506250000001</v>
       </c>
       <c r="V4" s="6" t="s">
@@ -4731,27 +4731,27 @@
         <v>0.38900000000000001</v>
       </c>
       <c r="N5">
-        <f>L5/'Non insulated v4 TUV'!$X$1</f>
+        <f>L5/Data!$X$1</f>
         <v>376.20030975735676</v>
       </c>
       <c r="P5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.63</v>
       </c>
       <c r="R5">
-        <f>S5*Q5</f>
+        <f t="shared" si="0"/>
         <v>973.72800000000007</v>
       </c>
       <c r="S5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="T5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.15752961000000001</v>
       </c>
       <c r="V5" s="9" cm="1">
@@ -4816,27 +4816,27 @@
         <v>0.38800000000000001</v>
       </c>
       <c r="N6">
-        <f>L6/'Non insulated v4 TUV'!$X$1</f>
+        <f>L6/Data!$X$1</f>
         <v>375.11615900877644</v>
       </c>
       <c r="P6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.43</v>
       </c>
       <c r="R6">
-        <f>S6*Q6</f>
+        <f t="shared" si="0"/>
         <v>664.60800000000006</v>
       </c>
       <c r="S6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="T6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4188009999999991E-2</v>
       </c>
       <c r="V6" s="6">
@@ -4900,27 +4900,27 @@
         <v>0.34300000000000003</v>
       </c>
       <c r="N7">
-        <f>L7/'Non insulated v4 TUV'!$X$1</f>
+        <f>L7/Data!$X$1</f>
         <v>331.75012906556532</v>
       </c>
       <c r="P7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.03</v>
       </c>
       <c r="R7">
-        <f>S7*Q7</f>
+        <f t="shared" si="0"/>
         <v>8.6939999999999955</v>
       </c>
       <c r="S7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="T7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.0999999999999997E-7</v>
       </c>
       <c r="V7" s="16">
@@ -4984,27 +4984,27 @@
         <v>0.34200000000000003</v>
       </c>
       <c r="N8">
-        <f>L8/'Non insulated v4 TUV'!$X$1</f>
+        <f>L8/Data!$X$1</f>
         <v>330.66597831698505</v>
       </c>
       <c r="P8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.14000000000000001</v>
       </c>
       <c r="R8">
-        <f>S8*Q8</f>
+        <f t="shared" si="0"/>
         <v>40.571999999999981</v>
       </c>
       <c r="S8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="T8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.8416000000000009E-4</v>
       </c>
       <c r="V8" s="6">
@@ -5068,27 +5068,27 @@
         <v>0.34200000000000003</v>
       </c>
       <c r="N9">
-        <f>L9/'Non insulated v4 TUV'!$X$1</f>
+        <f>L9/Data!$X$1</f>
         <v>330.30459473412492</v>
       </c>
       <c r="P9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.06</v>
       </c>
       <c r="R9">
-        <f>S9*Q9</f>
+        <f t="shared" si="0"/>
         <v>-13464.107999999998</v>
       </c>
       <c r="S9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2221.7999999999997</v>
       </c>
       <c r="T9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1348.6227969599997</v>
       </c>
       <c r="V9" s="13">
@@ -5152,27 +5152,27 @@
         <v>0.34200000000000003</v>
       </c>
       <c r="N10">
-        <f>L10/'Non insulated v4 TUV'!$X$1</f>
+        <f>L10/Data!$X$1</f>
         <v>330.35622096024781</v>
       </c>
       <c r="P10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.11</v>
       </c>
       <c r="R10">
-        <f>S10*Q10</f>
+        <f t="shared" si="0"/>
         <v>-13575.197999999999</v>
       </c>
       <c r="S10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2221.7999999999997</v>
       </c>
       <c r="T10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1393.6856904100002</v>
       </c>
     </row>
@@ -5217,27 +5217,27 @@
         <v>0.30499999999999999</v>
       </c>
       <c r="N11">
-        <f>L11/'Non insulated v4 TUV'!$X$1</f>
+        <f>L11/Data!$X$1</f>
         <v>294.83737738771293</v>
       </c>
       <c r="P11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.95</v>
       </c>
       <c r="R11">
-        <f>S11*Q11</f>
+        <f t="shared" si="0"/>
         <v>-10741.920000000002</v>
       </c>
       <c r="S11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="T11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2333.1315062500003</v>
       </c>
       <c r="AC11" s="27" t="s">
@@ -5285,27 +5285,27 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="N12">
-        <f>L12/'Non insulated v4 TUV'!$X$1</f>
+        <f>L12/Data!$X$1</f>
         <v>295.76664945792459</v>
       </c>
       <c r="P12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.79</v>
       </c>
       <c r="R12">
-        <f>S12*Q12</f>
+        <f t="shared" si="0"/>
         <v>-10494.624000000002</v>
       </c>
       <c r="S12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="T12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2125.5880368100002</v>
       </c>
       <c r="V12" t="s">
@@ -5371,27 +5371,27 @@
         <v>0.247</v>
       </c>
       <c r="N13">
-        <f>L13/'Non insulated v4 TUV'!$X$1</f>
+        <f>L13/Data!$X$1</f>
         <v>238.51316468766132</v>
       </c>
       <c r="P13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.23</v>
       </c>
       <c r="R13">
-        <f>S13*Q13</f>
+        <f t="shared" si="0"/>
         <v>-2095.253999999999</v>
       </c>
       <c r="S13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="T13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2732.4560744100008</v>
       </c>
       <c r="V13" s="27" t="s">
@@ -5457,27 +5457,27 @@
         <v>0.248</v>
       </c>
       <c r="N14">
-        <f>L14/'Non insulated v4 TUV'!$X$1</f>
+        <f>L14/Data!$X$1</f>
         <v>239.28755807950438</v>
       </c>
       <c r="P14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.23</v>
       </c>
       <c r="R14">
-        <f>S14*Q14</f>
+        <f t="shared" si="0"/>
         <v>-2095.253999999999</v>
       </c>
       <c r="S14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="T14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2732.4560744100008</v>
       </c>
     </row>
@@ -5522,27 +5522,27 @@
         <v>0.252</v>
       </c>
       <c r="N15">
-        <f>L15/'Non insulated v4 TUV'!$X$1</f>
+        <f>L15/Data!$X$1</f>
         <v>243.21115126484256</v>
       </c>
       <c r="P15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.97</v>
       </c>
       <c r="R15">
-        <f>S15*Q15</f>
+        <f t="shared" si="0"/>
         <v>-33260.345999999998</v>
       </c>
       <c r="S15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2221.7999999999997</v>
       </c>
       <c r="T15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50221.213380810012</v>
       </c>
     </row>
@@ -5587,27 +5587,27 @@
         <v>0.252</v>
       </c>
       <c r="N16">
-        <f>L16/'Non insulated v4 TUV'!$X$1</f>
+        <f>L16/Data!$X$1</f>
         <v>243.88229220443984</v>
       </c>
       <c r="P16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.8</v>
       </c>
       <c r="R16">
-        <f>S16*Q16</f>
+        <f t="shared" si="0"/>
         <v>-32882.639999999999</v>
       </c>
       <c r="S16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2221.7999999999997</v>
       </c>
       <c r="T16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47978.521600000007</v>
       </c>
     </row>
@@ -5652,27 +5652,27 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="N17">
-        <f>L17/'Non insulated v4 TUV'!$X$1</f>
+        <f>L17/Data!$X$1</f>
         <v>197.88332472896232</v>
       </c>
       <c r="P17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.74</v>
       </c>
       <c r="R17">
-        <f>S17*Q17</f>
+        <f t="shared" si="0"/>
         <v>-24327.744000000002</v>
       </c>
       <c r="S17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="T17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61378.873305760004</v>
       </c>
     </row>
@@ -5717,27 +5717,27 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="N18">
-        <f>L18/'Non insulated v4 TUV'!$X$1</f>
+        <f>L18/Data!$X$1</f>
         <v>198.29633453794528</v>
       </c>
       <c r="P18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.65</v>
       </c>
       <c r="R18">
-        <f>S18*Q18</f>
+        <f t="shared" si="0"/>
         <v>-24188.640000000003</v>
       </c>
       <c r="S18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1545.6000000000001</v>
       </c>
       <c r="T18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59987.031006250007</v>
       </c>
     </row>
@@ -5782,27 +5782,27 @@
         <v>0.127</v>
       </c>
       <c r="N19">
-        <f>L19/'Non insulated v4 TUV'!$X$1</f>
+        <f>L19/Data!$X$1</f>
         <v>122.71553949406298</v>
       </c>
       <c r="P19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.14</v>
       </c>
       <c r="R19">
-        <f>S19*Q19</f>
+        <f t="shared" si="0"/>
         <v>-4677.3719999999976</v>
       </c>
       <c r="S19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="T19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67860.041600160024</v>
       </c>
     </row>
@@ -5847,27 +5847,27 @@
         <v>0.127</v>
       </c>
       <c r="N20">
-        <f>L20/'Non insulated v4 TUV'!$X$1</f>
+        <f>L20/Data!$X$1</f>
         <v>122.8704181724316</v>
       </c>
       <c r="P20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>966</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.18</v>
       </c>
       <c r="R20">
-        <f>S20*Q20</f>
+        <f t="shared" si="0"/>
         <v>-4688.9639999999972</v>
       </c>
       <c r="S20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-289.79999999999984</v>
       </c>
       <c r="T20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68535.260697759993</v>
       </c>
     </row>

</xml_diff>